<commit_message>
Add fonts and maj liste_params
</commit_message>
<xml_diff>
--- a/doc/Liste_params.xlsx
+++ b/doc/Liste_params.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
   <si>
     <t>Nom</t>
   </si>
@@ -146,6 +146,12 @@
   <si>
     <t>Temps de spawn en seconde d'un zombie dans un village
 A chaque itération un zombie est créé pour un humain mort</t>
+  </si>
+  <si>
+    <t>Nbr_Sign_Life</t>
+  </si>
+  <si>
+    <t>Nombre de zombies qui peuvent passer sur un panneau avant de la casser</t>
   </si>
 </sst>
 </file>
@@ -508,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D20"/>
+  <dimension ref="A2:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,6 +792,20 @@
       </c>
       <c r="D20" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="4">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>